<commit_message>
Přidání null checků, další funkcionalita, finish projektu
</commit_message>
<xml_diff>
--- a/SourceData/data.xlsx
+++ b/SourceData/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="List 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="DATA" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -74,34 +74,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-    </font>
+    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,14 +96,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -360,10 +343,10 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -374,7 +357,7 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -388,7 +371,7 @@
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -402,10 +385,10 @@
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>